<commit_message>
finds group of professor
</commit_message>
<xml_diff>
--- a/rasa/data/info.xlsx
+++ b/rasa/data/info.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">NOMBRE</t>
   </si>
   <si>
-    <t xml:space="preserve">GRUPO </t>
+    <t xml:space="preserve">GRUPO</t>
   </si>
   <si>
     <t xml:space="preserve">DESPACHO</t>
@@ -865,7 +865,6 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -873,6 +872,7 @@
       <charset val="1"/>
     </font>
     <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -949,12 +949,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -965,15 +969,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1057,13 +1057,13 @@
   <dimension ref="A1:X879"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B:D"/>
+      <selection pane="topLeft" activeCell="A52" activeCellId="0" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="67.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="50.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="69.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.5"/>
   </cols>
@@ -1101,9 +1101,9 @@
       <c r="X1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
+      <c r="A2" s="5"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
@@ -1133,7 +1133,7 @@
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5" t="n">
+      <c r="C3" s="4" t="n">
         <v>55110</v>
       </c>
       <c r="D3" s="3"/>
@@ -1165,7 +1165,7 @@
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="n">
+      <c r="C4" s="4" t="n">
         <v>55130</v>
       </c>
       <c r="D4" s="3"/>
@@ -1197,7 +1197,7 @@
       <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="4" t="n">
         <v>55130</v>
       </c>
       <c r="D5" s="3"/>
@@ -1229,7 +1229,7 @@
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="5" t="n">
+      <c r="C6" s="4" t="n">
         <v>55130</v>
       </c>
       <c r="D6" s="3"/>
@@ -1261,7 +1261,7 @@
       <c r="B7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="5" t="n">
+      <c r="C7" s="4" t="n">
         <v>55130</v>
       </c>
       <c r="D7" s="3"/>
@@ -1293,7 +1293,7 @@
       <c r="B8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="5" t="n">
+      <c r="C8" s="4" t="n">
         <v>55130</v>
       </c>
       <c r="D8" s="3"/>
@@ -1325,7 +1325,7 @@
       <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="5" t="n">
+      <c r="C9" s="4" t="n">
         <v>55200</v>
       </c>
       <c r="D9" s="3"/>
@@ -1357,7 +1357,7 @@
       <c r="B10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="5" t="n">
+      <c r="C10" s="4" t="n">
         <v>55201</v>
       </c>
       <c r="D10" s="3"/>
@@ -1389,7 +1389,7 @@
       <c r="B11" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5" t="n">
+      <c r="C11" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D11" s="3"/>
@@ -1421,7 +1421,7 @@
       <c r="B12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="5" t="n">
+      <c r="C12" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D12" s="3"/>
@@ -1453,7 +1453,7 @@
       <c r="B13" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5" t="n">
+      <c r="C13" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D13" s="3"/>
@@ -1485,7 +1485,7 @@
       <c r="B14" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="5" t="n">
+      <c r="C14" s="4" t="n">
         <v>55217</v>
       </c>
       <c r="D14" s="3"/>
@@ -1517,7 +1517,7 @@
       <c r="B15" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5" t="n">
+      <c r="C15" s="4" t="n">
         <v>55217</v>
       </c>
       <c r="D15" s="3"/>
@@ -1549,7 +1549,7 @@
       <c r="B16" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="5" t="n">
+      <c r="C16" s="4" t="n">
         <v>55217</v>
       </c>
       <c r="D16" s="3"/>
@@ -1581,7 +1581,7 @@
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="5" t="n">
+      <c r="C17" s="4" t="n">
         <v>55219</v>
       </c>
       <c r="D17" s="3"/>
@@ -1613,7 +1613,7 @@
       <c r="B18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="5" t="n">
+      <c r="C18" s="4" t="n">
         <v>55219</v>
       </c>
       <c r="D18" s="3"/>
@@ -1642,10 +1642,10 @@
       <c r="A19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="5" t="n">
+      <c r="C19" s="4" t="n">
         <v>51008</v>
       </c>
       <c r="D19" s="3" t="s">
@@ -1676,10 +1676,10 @@
       <c r="A20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="5" t="n">
+      <c r="C20" s="4" t="n">
         <v>51014</v>
       </c>
       <c r="D20" s="3" t="s">
@@ -1707,13 +1707,13 @@
       <c r="X20" s="3"/>
     </row>
     <row r="21" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C21" s="5" t="n">
+      <c r="C21" s="4" t="n">
         <v>51014</v>
       </c>
       <c r="D21" s="3" t="s">
@@ -1744,10 +1744,10 @@
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="5" t="n">
+      <c r="C22" s="4" t="n">
         <v>51014</v>
       </c>
       <c r="D22" s="3" t="s">
@@ -1778,10 +1778,10 @@
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="5" t="n">
+      <c r="C23" s="4" t="n">
         <v>51014</v>
       </c>
       <c r="D23" s="3" t="s">
@@ -1812,10 +1812,10 @@
       <c r="A24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="5" t="n">
+      <c r="C24" s="4" t="n">
         <v>51015</v>
       </c>
       <c r="D24" s="3" t="s">
@@ -1846,10 +1846,10 @@
       <c r="A25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="5" t="n">
+      <c r="C25" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D25" s="3" t="s">
@@ -1880,10 +1880,10 @@
       <c r="A26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="5" t="n">
+      <c r="C26" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D26" s="3" t="s">
@@ -1914,10 +1914,10 @@
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C27" s="5" t="n">
+      <c r="C27" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D27" s="3" t="s">
@@ -1948,10 +1948,10 @@
       <c r="A28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="5" t="n">
+      <c r="C28" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D28" s="3" t="s">
@@ -1982,10 +1982,10 @@
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="5" t="n">
+      <c r="C29" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D29" s="3" t="s">
@@ -2016,10 +2016,10 @@
       <c r="A30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="5" t="n">
+      <c r="C30" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D30" s="3"/>
@@ -2048,10 +2048,10 @@
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="5" t="n">
+      <c r="C31" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D31" s="3"/>
@@ -2080,10 +2080,10 @@
       <c r="A32" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C32" s="5" t="n">
+      <c r="C32" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D32" s="3"/>
@@ -2112,10 +2112,10 @@
       <c r="A33" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="5" t="n">
+      <c r="C33" s="4" t="n">
         <v>51017</v>
       </c>
       <c r="D33" s="8" t="s">
@@ -2149,7 +2149,7 @@
       <c r="B34" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="5" t="n">
+      <c r="C34" s="4" t="n">
         <v>51100</v>
       </c>
       <c r="D34" s="3" t="s">
@@ -2183,7 +2183,7 @@
       <c r="B35" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C35" s="5" t="n">
+      <c r="C35" s="4" t="n">
         <v>51100</v>
       </c>
       <c r="D35" s="3" t="s">
@@ -2217,7 +2217,7 @@
       <c r="B36" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="5" t="n">
+      <c r="C36" s="4" t="n">
         <v>51107</v>
       </c>
       <c r="D36" s="3" t="s">
@@ -2251,7 +2251,7 @@
       <c r="B37" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C37" s="5" t="n">
+      <c r="C37" s="4" t="n">
         <v>51107</v>
       </c>
       <c r="D37" s="3" t="s">
@@ -2285,7 +2285,7 @@
       <c r="B38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="5" t="n">
+      <c r="C38" s="4" t="n">
         <v>51107</v>
       </c>
       <c r="D38" s="3" t="s">
@@ -2319,7 +2319,7 @@
       <c r="B39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C39" s="5" t="n">
+      <c r="C39" s="4" t="n">
         <v>51107</v>
       </c>
       <c r="D39" s="3" t="s">
@@ -2353,7 +2353,7 @@
       <c r="B40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="5" t="n">
+      <c r="C40" s="4" t="n">
         <v>55108</v>
       </c>
       <c r="D40" s="3"/>
@@ -2385,7 +2385,7 @@
       <c r="B41" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="5" t="n">
+      <c r="C41" s="4" t="n">
         <v>55108</v>
       </c>
       <c r="D41" s="3"/>
@@ -2417,7 +2417,7 @@
       <c r="B42" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="5" t="n">
+      <c r="C42" s="4" t="n">
         <v>55122</v>
       </c>
       <c r="D42" s="3"/>
@@ -2449,7 +2449,7 @@
       <c r="B43" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="5" t="n">
+      <c r="C43" s="4" t="n">
         <v>55124</v>
       </c>
       <c r="D43" s="3"/>
@@ -2481,7 +2481,7 @@
       <c r="B44" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="5" t="n">
+      <c r="C44" s="4" t="n">
         <v>55124</v>
       </c>
       <c r="D44" s="3"/>
@@ -2513,7 +2513,7 @@
       <c r="B45" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C45" s="5" t="n">
+      <c r="C45" s="4" t="n">
         <v>55124</v>
       </c>
       <c r="D45" s="3"/>
@@ -2545,7 +2545,7 @@
       <c r="B46" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C46" s="5" t="n">
+      <c r="C46" s="4" t="n">
         <v>55124</v>
       </c>
       <c r="D46" s="3"/>
@@ -2577,7 +2577,7 @@
       <c r="B47" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="5" t="n">
+      <c r="C47" s="4" t="n">
         <v>55220</v>
       </c>
       <c r="D47" s="3"/>
@@ -2609,7 +2609,7 @@
       <c r="B48" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C48" s="5" t="n">
+      <c r="C48" s="4" t="n">
         <v>55312</v>
       </c>
       <c r="D48" s="3"/>
@@ -2638,10 +2638,10 @@
       <c r="A49" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C49" s="5" t="n">
+      <c r="C49" s="4" t="n">
         <v>55422</v>
       </c>
       <c r="D49" s="3"/>
@@ -2670,10 +2670,10 @@
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C50" s="5" t="n">
+      <c r="C50" s="4" t="n">
         <v>55203</v>
       </c>
       <c r="D50" s="3"/>
@@ -2702,10 +2702,10 @@
       <c r="A51" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C51" s="5" t="n">
+      <c r="C51" s="4" t="n">
         <v>55205</v>
       </c>
       <c r="D51" s="3"/>
@@ -2734,10 +2734,10 @@
       <c r="A52" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C52" s="5" t="n">
+      <c r="C52" s="4" t="n">
         <v>55205</v>
       </c>
       <c r="D52" s="3"/>
@@ -2766,10 +2766,10 @@
       <c r="A53" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C53" s="5" t="n">
+      <c r="C53" s="4" t="n">
         <v>55205</v>
       </c>
       <c r="D53" s="3"/>
@@ -2798,10 +2798,10 @@
       <c r="A54" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C54" s="5" t="n">
+      <c r="C54" s="4" t="n">
         <v>55205</v>
       </c>
       <c r="D54" s="3"/>
@@ -2830,10 +2830,10 @@
       <c r="A55" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C55" s="5" t="n">
+      <c r="C55" s="4" t="n">
         <v>55205</v>
       </c>
       <c r="D55" s="3"/>
@@ -2862,10 +2862,10 @@
       <c r="A56" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C56" s="5" t="n">
+      <c r="C56" s="4" t="n">
         <v>55221</v>
       </c>
       <c r="D56" s="3"/>
@@ -2897,7 +2897,7 @@
       <c r="B57" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="5" t="n">
+      <c r="C57" s="4" t="n">
         <v>55116</v>
       </c>
       <c r="D57" s="3"/>
@@ -2929,7 +2929,7 @@
       <c r="B58" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C58" s="5" t="n">
+      <c r="C58" s="4" t="n">
         <v>55116</v>
       </c>
       <c r="D58" s="3"/>
@@ -2961,7 +2961,7 @@
       <c r="B59" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C59" s="5" t="n">
+      <c r="C59" s="4" t="n">
         <v>55116</v>
       </c>
       <c r="D59" s="3"/>
@@ -2993,7 +2993,7 @@
       <c r="B60" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C60" s="5" t="n">
+      <c r="C60" s="4" t="n">
         <v>55118</v>
       </c>
       <c r="D60" s="3"/>
@@ -3025,7 +3025,7 @@
       <c r="B61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C61" s="5" t="n">
+      <c r="C61" s="4" t="n">
         <v>55118</v>
       </c>
       <c r="D61" s="3"/>
@@ -3057,7 +3057,7 @@
       <c r="B62" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C62" s="5" t="n">
+      <c r="C62" s="4" t="n">
         <v>55120</v>
       </c>
       <c r="D62" s="3"/>
@@ -3089,7 +3089,7 @@
       <c r="B63" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C63" s="5" t="n">
+      <c r="C63" s="4" t="n">
         <v>55424</v>
       </c>
       <c r="D63" s="3"/>
@@ -3121,7 +3121,7 @@
       <c r="B64" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="5" t="n">
+      <c r="C64" s="4" t="n">
         <v>55120</v>
       </c>
       <c r="D64" s="3"/>
@@ -3153,7 +3153,7 @@
       <c r="B65" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C65" s="5" t="n">
+      <c r="C65" s="4" t="n">
         <v>55120</v>
       </c>
       <c r="D65" s="3"/>
@@ -3185,7 +3185,7 @@
       <c r="B66" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C66" s="5" t="n">
+      <c r="C66" s="4" t="n">
         <v>55120</v>
       </c>
       <c r="D66" s="3"/>
@@ -3217,7 +3217,7 @@
       <c r="B67" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C67" s="5" t="n">
+      <c r="C67" s="4" t="n">
         <v>55204</v>
       </c>
       <c r="D67" s="3"/>
@@ -3249,7 +3249,7 @@
       <c r="B68" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C68" s="5" t="n">
+      <c r="C68" s="4" t="n">
         <v>55204</v>
       </c>
       <c r="D68" s="3"/>
@@ -3281,7 +3281,7 @@
       <c r="B69" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C69" s="5" t="n">
+      <c r="C69" s="4" t="n">
         <v>55206</v>
       </c>
       <c r="D69" s="3"/>
@@ -3313,7 +3313,7 @@
       <c r="B70" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C70" s="5" t="n">
+      <c r="C70" s="4" t="n">
         <v>55206</v>
       </c>
       <c r="D70" s="3"/>
@@ -3345,7 +3345,7 @@
       <c r="B71" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C71" s="5" t="n">
+      <c r="C71" s="4" t="n">
         <v>55208</v>
       </c>
       <c r="D71" s="3"/>
@@ -3377,7 +3377,7 @@
       <c r="B72" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C72" s="5" t="n">
+      <c r="C72" s="4" t="n">
         <v>55222</v>
       </c>
       <c r="D72" s="3"/>
@@ -3409,7 +3409,7 @@
       <c r="B73" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C73" s="5" t="n">
+      <c r="C73" s="4" t="n">
         <v>55102</v>
       </c>
       <c r="D73" s="3"/>
@@ -3441,7 +3441,7 @@
       <c r="B74" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C74" s="5" t="n">
+      <c r="C74" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D74" s="3"/>
@@ -3473,7 +3473,7 @@
       <c r="B75" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C75" s="5" t="n">
+      <c r="C75" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D75" s="3"/>
@@ -3505,7 +3505,7 @@
       <c r="B76" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C76" s="5" t="n">
+      <c r="C76" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D76" s="3"/>
@@ -3537,7 +3537,7 @@
       <c r="B77" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C77" s="5" t="n">
+      <c r="C77" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D77" s="3"/>
@@ -3569,7 +3569,7 @@
       <c r="B78" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C78" s="5" t="n">
+      <c r="C78" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D78" s="3"/>
@@ -3601,7 +3601,7 @@
       <c r="B79" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C79" s="5" t="n">
+      <c r="C79" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D79" s="3"/>
@@ -3633,7 +3633,7 @@
       <c r="B80" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C80" s="5" t="n">
+      <c r="C80" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D80" s="3"/>
@@ -3665,7 +3665,7 @@
       <c r="B81" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C81" s="5" t="n">
+      <c r="C81" s="4" t="n">
         <v>55112</v>
       </c>
       <c r="D81" s="3"/>
@@ -3697,7 +3697,7 @@
       <c r="B82" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="C82" s="5" t="n">
+      <c r="C82" s="4" t="n">
         <v>55126</v>
       </c>
       <c r="D82" s="3"/>
@@ -3725,7 +3725,7 @@
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
-      <c r="C83" s="5"/>
+      <c r="C83" s="4"/>
       <c r="D83" s="3"/>
       <c r="E83" s="3"/>
       <c r="F83" s="3"/>
@@ -3755,7 +3755,7 @@
       <c r="B84" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C84" s="5" t="n">
+      <c r="C84" s="4" t="n">
         <v>55300</v>
       </c>
       <c r="D84" s="3"/>
@@ -3787,7 +3787,7 @@
       <c r="B85" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C85" s="5" t="n">
+      <c r="C85" s="4" t="n">
         <v>55301</v>
       </c>
       <c r="D85" s="3"/>
@@ -3819,7 +3819,7 @@
       <c r="B86" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C86" s="5" t="n">
+      <c r="C86" s="4" t="n">
         <v>55302</v>
       </c>
       <c r="D86" s="3"/>
@@ -3851,7 +3851,7 @@
       <c r="B87" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C87" s="5" t="n">
+      <c r="C87" s="4" t="n">
         <v>55302</v>
       </c>
       <c r="D87" s="3"/>
@@ -3883,7 +3883,7 @@
       <c r="B88" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C88" s="5" t="n">
+      <c r="C88" s="4" t="n">
         <v>55302</v>
       </c>
       <c r="D88" s="3"/>
@@ -3915,7 +3915,7 @@
       <c r="B89" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C89" s="5" t="n">
+      <c r="C89" s="4" t="n">
         <v>55302</v>
       </c>
       <c r="D89" s="3"/>
@@ -3947,7 +3947,7 @@
       <c r="B90" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C90" s="5" t="n">
+      <c r="C90" s="4" t="n">
         <v>55302</v>
       </c>
       <c r="D90" s="3"/>
@@ -3979,7 +3979,7 @@
       <c r="B91" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C91" s="5" t="n">
+      <c r="C91" s="4" t="n">
         <v>55305</v>
       </c>
       <c r="D91" s="3"/>
@@ -4011,7 +4011,7 @@
       <c r="B92" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C92" s="5" t="n">
+      <c r="C92" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D92" s="3"/>
@@ -4043,7 +4043,7 @@
       <c r="B93" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C93" s="5" t="n">
+      <c r="C93" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D93" s="3"/>
@@ -4075,7 +4075,7 @@
       <c r="B94" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C94" s="5" t="n">
+      <c r="C94" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D94" s="3"/>
@@ -4107,7 +4107,7 @@
       <c r="B95" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C95" s="5" t="n">
+      <c r="C95" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D95" s="3"/>
@@ -4139,7 +4139,7 @@
       <c r="B96" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C96" s="5" t="n">
+      <c r="C96" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D96" s="3"/>
@@ -4171,7 +4171,7 @@
       <c r="B97" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C97" s="5" t="n">
+      <c r="C97" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D97" s="3"/>
@@ -4203,7 +4203,7 @@
       <c r="B98" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C98" s="5" t="n">
+      <c r="C98" s="4" t="n">
         <v>55306</v>
       </c>
       <c r="D98" s="3"/>
@@ -4235,7 +4235,7 @@
       <c r="B99" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C99" s="5" t="n">
+      <c r="C99" s="4" t="n">
         <v>55308</v>
       </c>
       <c r="D99" s="3"/>
@@ -4267,7 +4267,7 @@
       <c r="B100" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C100" s="5" t="n">
+      <c r="C100" s="4" t="n">
         <v>55308</v>
       </c>
       <c r="D100" s="3"/>
@@ -4299,7 +4299,7 @@
       <c r="B101" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C101" s="5" t="n">
+      <c r="C101" s="4" t="n">
         <v>55308</v>
       </c>
       <c r="D101" s="3"/>
@@ -4331,7 +4331,7 @@
       <c r="B102" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C102" s="5" t="n">
+      <c r="C102" s="4" t="n">
         <v>55308</v>
       </c>
       <c r="D102" s="3"/>
@@ -4363,7 +4363,7 @@
       <c r="B103" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C103" s="5" t="n">
+      <c r="C103" s="4" t="n">
         <v>55310</v>
       </c>
       <c r="D103" s="3"/>
@@ -4395,7 +4395,7 @@
       <c r="B104" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C104" s="5" t="n">
+      <c r="C104" s="4" t="n">
         <v>55310</v>
       </c>
       <c r="D104" s="3"/>
@@ -4427,7 +4427,7 @@
       <c r="B105" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C105" s="5" t="n">
+      <c r="C105" s="4" t="n">
         <v>55310</v>
       </c>
       <c r="D105" s="3"/>
@@ -4459,7 +4459,7 @@
       <c r="B106" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C106" s="5" t="n">
+      <c r="C106" s="4" t="n">
         <v>55312</v>
       </c>
       <c r="D106" s="3"/>
@@ -4491,7 +4491,7 @@
       <c r="B107" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C107" s="5" t="n">
+      <c r="C107" s="4" t="n">
         <v>55312</v>
       </c>
       <c r="D107" s="3"/>
@@ -4523,7 +4523,7 @@
       <c r="B108" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C108" s="5" t="n">
+      <c r="C108" s="4" t="n">
         <v>55312</v>
       </c>
       <c r="D108" s="3"/>
@@ -4555,7 +4555,7 @@
       <c r="B109" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C109" s="5" t="n">
+      <c r="C109" s="4" t="n">
         <v>55314</v>
       </c>
       <c r="D109" s="3"/>
@@ -4587,7 +4587,7 @@
       <c r="B110" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C110" s="5" t="n">
+      <c r="C110" s="4" t="n">
         <v>55314</v>
       </c>
       <c r="D110" s="3"/>
@@ -4619,7 +4619,7 @@
       <c r="B111" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C111" s="5" t="n">
+      <c r="C111" s="4" t="n">
         <v>55314</v>
       </c>
       <c r="D111" s="3"/>
@@ -4651,7 +4651,7 @@
       <c r="B112" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C112" s="5" t="n">
+      <c r="C112" s="4" t="n">
         <v>55316</v>
       </c>
       <c r="D112" s="3"/>
@@ -4683,7 +4683,7 @@
       <c r="B113" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C113" s="5" t="n">
+      <c r="C113" s="4" t="n">
         <v>55316</v>
       </c>
       <c r="D113" s="3"/>
@@ -4715,7 +4715,7 @@
       <c r="B114" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C114" s="5" t="n">
+      <c r="C114" s="4" t="n">
         <v>55316</v>
       </c>
       <c r="D114" s="3"/>
@@ -4747,7 +4747,7 @@
       <c r="B115" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C115" s="5" t="n">
+      <c r="C115" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D115" s="3"/>
@@ -4779,7 +4779,7 @@
       <c r="B116" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C116" s="5" t="n">
+      <c r="C116" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D116" s="3"/>
@@ -4811,7 +4811,7 @@
       <c r="B117" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C117" s="5" t="n">
+      <c r="C117" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D117" s="3"/>
@@ -4843,7 +4843,7 @@
       <c r="B118" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C118" s="5" t="n">
+      <c r="C118" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D118" s="3"/>
@@ -4875,7 +4875,7 @@
       <c r="B119" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C119" s="5" t="n">
+      <c r="C119" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D119" s="3"/>
@@ -4907,7 +4907,7 @@
       <c r="B120" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C120" s="5" t="n">
+      <c r="C120" s="4" t="n">
         <v>55320</v>
       </c>
       <c r="D120" s="3"/>
@@ -4939,7 +4939,7 @@
       <c r="B121" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C121" s="5" t="n">
+      <c r="C121" s="4" t="n">
         <v>55320</v>
       </c>
       <c r="D121" s="3"/>
@@ -4971,7 +4971,7 @@
       <c r="B122" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C122" s="5" t="n">
+      <c r="C122" s="4" t="n">
         <v>55322</v>
       </c>
       <c r="D122" s="3"/>
@@ -5003,7 +5003,7 @@
       <c r="B123" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C123" s="5" t="n">
+      <c r="C123" s="4" t="n">
         <v>55322</v>
       </c>
       <c r="D123" s="3"/>
@@ -5035,7 +5035,7 @@
       <c r="B124" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C124" s="5" t="n">
+      <c r="C124" s="4" t="n">
         <v>55324</v>
       </c>
       <c r="D124" s="3"/>
@@ -5067,7 +5067,7 @@
       <c r="B125" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C125" s="5" t="n">
+      <c r="C125" s="4" t="n">
         <v>55326</v>
       </c>
       <c r="D125" s="3"/>
@@ -5099,7 +5099,7 @@
       <c r="B126" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C126" s="5" t="n">
+      <c r="C126" s="4" t="n">
         <v>51005</v>
       </c>
       <c r="D126" s="3" t="s">
@@ -5133,7 +5133,7 @@
       <c r="B127" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="C127" s="5" t="n">
+      <c r="C127" s="4" t="n">
         <v>55318</v>
       </c>
       <c r="D127" s="3"/>
@@ -5165,7 +5165,7 @@
       <c r="B128" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="C128" s="5" t="n">
+      <c r="C128" s="4" t="n">
         <v>55418</v>
       </c>
       <c r="D128" s="3"/>
@@ -5194,10 +5194,10 @@
       <c r="A129" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B129" s="7" t="s">
+      <c r="B129" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C129" s="5" t="n">
+      <c r="C129" s="4" t="n">
         <v>55422</v>
       </c>
       <c r="D129" s="3"/>
@@ -5229,7 +5229,7 @@
       <c r="B130" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C130" s="5" t="n">
+      <c r="C130" s="4" t="n">
         <v>55226</v>
       </c>
       <c r="D130" s="3"/>
@@ -5261,7 +5261,7 @@
       <c r="B131" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C131" s="5" t="n">
+      <c r="C131" s="4" t="n">
         <v>55100</v>
       </c>
       <c r="D131" s="3"/>
@@ -5293,7 +5293,7 @@
       <c r="B132" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C132" s="5" t="n">
+      <c r="C132" s="4" t="n">
         <v>55117</v>
       </c>
       <c r="D132" s="3"/>
@@ -5325,7 +5325,7 @@
       <c r="B133" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C133" s="5" t="n">
+      <c r="C133" s="4" t="n">
         <v>55117</v>
       </c>
       <c r="D133" s="3"/>
@@ -5357,7 +5357,7 @@
       <c r="B134" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C134" s="5" t="n">
+      <c r="C134" s="4" t="n">
         <v>55117</v>
       </c>
       <c r="D134" s="3"/>
@@ -5389,7 +5389,7 @@
       <c r="B135" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C135" s="5" t="n">
+      <c r="C135" s="4" t="n">
         <v>55117</v>
       </c>
       <c r="D135" s="3"/>
@@ -5421,7 +5421,7 @@
       <c r="B136" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="C136" s="5" t="n">
+      <c r="C136" s="4" t="n">
         <v>55117</v>
       </c>
       <c r="D136" s="3"/>
@@ -5453,7 +5453,7 @@
       <c r="B137" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C137" s="5" t="n">
+      <c r="C137" s="4" t="n">
         <v>55115</v>
       </c>
       <c r="D137" s="3"/>
@@ -5485,7 +5485,7 @@
       <c r="B138" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C138" s="5" t="n">
+      <c r="C138" s="4" t="n">
         <v>55115</v>
       </c>
       <c r="D138" s="3"/>
@@ -5517,7 +5517,7 @@
       <c r="B139" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C139" s="5" t="n">
+      <c r="C139" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D139" s="3"/>
@@ -5549,7 +5549,7 @@
       <c r="B140" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C140" s="5" t="n">
+      <c r="C140" s="4" t="n">
         <v>55121</v>
       </c>
       <c r="D140" s="3"/>
@@ -5581,7 +5581,7 @@
       <c r="B141" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C141" s="5" t="n">
+      <c r="C141" s="4" t="n">
         <v>55121</v>
       </c>
       <c r="D141" s="3"/>
@@ -5613,7 +5613,7 @@
       <c r="B142" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C142" s="5" t="n">
+      <c r="C142" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D142" s="3"/>
@@ -5645,7 +5645,7 @@
       <c r="B143" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C143" s="5" t="n">
+      <c r="C143" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D143" s="3"/>
@@ -5677,7 +5677,7 @@
       <c r="B144" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C144" s="5" t="n">
+      <c r="C144" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D144" s="3"/>
@@ -5709,7 +5709,7 @@
       <c r="B145" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C145" s="5" t="s">
+      <c r="C145" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D145" s="3"/>
@@ -5741,7 +5741,7 @@
       <c r="B146" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C146" s="5" t="s">
+      <c r="C146" s="4" t="s">
         <v>165</v>
       </c>
       <c r="D146" s="3"/>
@@ -5773,7 +5773,7 @@
       <c r="B147" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C147" s="5" t="n">
+      <c r="C147" s="4" t="n">
         <v>55223</v>
       </c>
       <c r="D147" s="3"/>
@@ -5805,7 +5805,7 @@
       <c r="B148" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C148" s="5" t="n">
+      <c r="C148" s="4" t="n">
         <v>55223</v>
       </c>
       <c r="D148" s="3"/>
@@ -5837,7 +5837,7 @@
       <c r="B149" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C149" s="5" t="n">
+      <c r="C149" s="4" t="n">
         <v>55223</v>
       </c>
       <c r="D149" s="3"/>
@@ -5869,7 +5869,7 @@
       <c r="B150" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C150" s="5" t="n">
+      <c r="C150" s="4" t="n">
         <v>55105</v>
       </c>
       <c r="D150" s="3"/>
@@ -5901,7 +5901,7 @@
       <c r="B151" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C151" s="5" t="n">
+      <c r="C151" s="4" t="n">
         <v>55107</v>
       </c>
       <c r="D151" s="3"/>
@@ -5933,7 +5933,7 @@
       <c r="B152" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C152" s="5" t="n">
+      <c r="C152" s="4" t="n">
         <v>55107</v>
       </c>
       <c r="D152" s="3"/>
@@ -5965,7 +5965,7 @@
       <c r="B153" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C153" s="5" t="n">
+      <c r="C153" s="4" t="n">
         <v>55109</v>
       </c>
       <c r="D153" s="3"/>
@@ -5997,7 +5997,7 @@
       <c r="B154" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C154" s="5" t="n">
+      <c r="C154" s="4" t="n">
         <v>55109</v>
       </c>
       <c r="D154" s="3"/>
@@ -6029,7 +6029,7 @@
       <c r="B155" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C155" s="5" t="n">
+      <c r="C155" s="4" t="n">
         <v>55109</v>
       </c>
       <c r="D155" s="3"/>
@@ -6061,7 +6061,7 @@
       <c r="B156" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C156" s="5" t="n">
+      <c r="C156" s="4" t="n">
         <v>55115</v>
       </c>
       <c r="D156" s="3"/>
@@ -6093,7 +6093,7 @@
       <c r="B157" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C157" s="5" t="n">
+      <c r="C157" s="4" t="n">
         <v>55115</v>
       </c>
       <c r="D157" s="3"/>
@@ -6125,7 +6125,7 @@
       <c r="B158" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C158" s="5" t="n">
+      <c r="C158" s="4" t="n">
         <v>55115</v>
       </c>
       <c r="D158" s="3"/>
@@ -6157,7 +6157,7 @@
       <c r="B159" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C159" s="5" t="n">
+      <c r="C159" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D159" s="3"/>
@@ -6189,7 +6189,7 @@
       <c r="B160" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C160" s="5" t="n">
+      <c r="C160" s="4" t="n">
         <v>55119</v>
       </c>
       <c r="D160" s="3"/>
@@ -6221,7 +6221,7 @@
       <c r="B161" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C161" s="5" t="n">
+      <c r="C161" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D161" s="3"/>
@@ -6253,7 +6253,7 @@
       <c r="B162" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C162" s="5" t="n">
+      <c r="C162" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D162" s="3"/>
@@ -6285,7 +6285,7 @@
       <c r="B163" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C163" s="5" t="n">
+      <c r="C163" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D163" s="3"/>
@@ -6317,7 +6317,7 @@
       <c r="B164" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C164" s="5" t="n">
+      <c r="C164" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D164" s="3"/>
@@ -6349,7 +6349,7 @@
       <c r="B165" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C165" s="5" t="n">
+      <c r="C165" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D165" s="3"/>
@@ -6381,7 +6381,7 @@
       <c r="B166" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C166" s="5" t="n">
+      <c r="C166" s="4" t="n">
         <v>55123</v>
       </c>
       <c r="D166" s="3"/>
@@ -6413,7 +6413,7 @@
       <c r="B167" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="C167" s="5" t="s">
+      <c r="C167" s="4" t="s">
         <v>163</v>
       </c>
       <c r="D167" s="3"/>
@@ -6445,7 +6445,7 @@
       <c r="B168" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C168" s="5" t="n">
+      <c r="C168" s="4" t="n">
         <v>55406</v>
       </c>
       <c r="D168" s="3"/>
@@ -6477,7 +6477,7 @@
       <c r="B169" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C169" s="5" t="n">
+      <c r="C169" s="4" t="n">
         <v>55408</v>
       </c>
       <c r="D169" s="3"/>
@@ -6509,7 +6509,7 @@
       <c r="B170" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C170" s="5" t="n">
+      <c r="C170" s="4" t="n">
         <v>55420</v>
       </c>
       <c r="D170" s="3"/>
@@ -6541,7 +6541,7 @@
       <c r="B171" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C171" s="5" t="n">
+      <c r="C171" s="4" t="n">
         <v>55301</v>
       </c>
       <c r="D171" s="3"/>
@@ -6573,7 +6573,7 @@
       <c r="B172" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C172" s="5" t="n">
+      <c r="C172" s="4" t="n">
         <v>55305</v>
       </c>
       <c r="D172" s="3"/>
@@ -6605,7 +6605,7 @@
       <c r="B173" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C173" s="5" t="n">
+      <c r="C173" s="4" t="n">
         <v>55400</v>
       </c>
       <c r="D173" s="3"/>
@@ -6637,7 +6637,7 @@
       <c r="B174" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C174" s="5" t="n">
+      <c r="C174" s="4" t="n">
         <v>55400</v>
       </c>
       <c r="D174" s="3"/>
@@ -6669,7 +6669,7 @@
       <c r="B175" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C175" s="5" t="n">
+      <c r="C175" s="4" t="n">
         <v>55402</v>
       </c>
       <c r="D175" s="3"/>
@@ -6697,7 +6697,7 @@
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="3"/>
       <c r="B176" s="3"/>
-      <c r="C176" s="5"/>
+      <c r="C176" s="4"/>
       <c r="D176" s="3"/>
       <c r="E176" s="3"/>
       <c r="F176" s="3"/>
@@ -6727,7 +6727,7 @@
       <c r="B177" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C177" s="5" t="n">
+      <c r="C177" s="4" t="n">
         <v>55402</v>
       </c>
       <c r="D177" s="3"/>
@@ -6759,7 +6759,7 @@
       <c r="B178" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C178" s="5" t="n">
+      <c r="C178" s="4" t="n">
         <v>55406</v>
       </c>
       <c r="D178" s="3"/>
@@ -6787,7 +6787,7 @@
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="3"/>
       <c r="B179" s="3"/>
-      <c r="C179" s="5"/>
+      <c r="C179" s="4"/>
       <c r="D179" s="3"/>
       <c r="E179" s="3"/>
       <c r="F179" s="3"/>
@@ -6813,7 +6813,7 @@
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="3"/>
       <c r="B180" s="3"/>
-      <c r="C180" s="5"/>
+      <c r="C180" s="4"/>
       <c r="D180" s="3"/>
       <c r="E180" s="3"/>
       <c r="F180" s="3"/>
@@ -6843,7 +6843,7 @@
       <c r="B181" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C181" s="5" t="n">
+      <c r="C181" s="4" t="n">
         <v>55416</v>
       </c>
       <c r="D181" s="3"/>
@@ -6875,7 +6875,7 @@
       <c r="B182" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C182" s="5" t="n">
+      <c r="C182" s="4" t="n">
         <v>55416</v>
       </c>
       <c r="D182" s="3"/>
@@ -6907,7 +6907,7 @@
       <c r="B183" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C183" s="5" t="n">
+      <c r="C183" s="4" t="n">
         <v>55420</v>
       </c>
       <c r="D183" s="3"/>
@@ -6939,7 +6939,7 @@
       <c r="B184" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C184" s="5" t="n">
+      <c r="C184" s="4" t="n">
         <v>55420</v>
       </c>
       <c r="D184" s="3"/>
@@ -6967,7 +6967,7 @@
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="3"/>
       <c r="B185" s="3"/>
-      <c r="C185" s="5"/>
+      <c r="C185" s="4"/>
       <c r="D185" s="3"/>
       <c r="E185" s="3"/>
       <c r="F185" s="3"/>
@@ -6997,7 +6997,7 @@
       <c r="B186" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C186" s="5" t="n">
+      <c r="C186" s="4" t="n">
         <v>55420</v>
       </c>
       <c r="D186" s="3"/>
@@ -7029,7 +7029,7 @@
       <c r="B187" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C187" s="5" t="n">
+      <c r="C187" s="4" t="n">
         <v>55424</v>
       </c>
       <c r="D187" s="3"/>
@@ -7061,7 +7061,7 @@
       <c r="B188" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C188" s="5" t="n">
+      <c r="C188" s="4" t="n">
         <v>55424</v>
       </c>
       <c r="D188" s="3"/>
@@ -7093,7 +7093,7 @@
       <c r="B189" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C189" s="5" t="n">
+      <c r="C189" s="4" t="n">
         <v>55424</v>
       </c>
       <c r="D189" s="3"/>
@@ -7125,7 +7125,7 @@
       <c r="B190" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C190" s="5" t="n">
+      <c r="C190" s="4" t="n">
         <v>55102</v>
       </c>
       <c r="D190" s="3"/>
@@ -7157,7 +7157,7 @@
       <c r="B191" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C191" s="5" t="n">
+      <c r="C191" s="4" t="n">
         <v>55102</v>
       </c>
       <c r="D191" s="3"/>
@@ -7189,7 +7189,7 @@
       <c r="B192" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C192" s="5" t="n">
+      <c r="C192" s="4" t="n">
         <v>55102</v>
       </c>
       <c r="D192" s="3"/>
@@ -7221,7 +7221,7 @@
       <c r="B193" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C193" s="5" t="n">
+      <c r="C193" s="4" t="n">
         <v>55102</v>
       </c>
       <c r="D193" s="3"/>
@@ -7253,7 +7253,7 @@
       <c r="B194" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C194" s="5" t="n">
+      <c r="C194" s="4" t="n">
         <v>55128</v>
       </c>
       <c r="D194" s="3"/>
@@ -7285,7 +7285,7 @@
       <c r="B195" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C195" s="5" t="n">
+      <c r="C195" s="4" t="n">
         <v>55128</v>
       </c>
       <c r="D195" s="3"/>
@@ -7317,7 +7317,7 @@
       <c r="B196" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C196" s="5" t="n">
+      <c r="C196" s="4" t="n">
         <v>55128</v>
       </c>
       <c r="D196" s="3"/>
@@ -7349,7 +7349,7 @@
       <c r="B197" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C197" s="5" t="n">
+      <c r="C197" s="4" t="n">
         <v>55008</v>
       </c>
       <c r="D197" s="3"/>
@@ -7381,7 +7381,7 @@
       <c r="B198" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C198" s="5" t="n">
+      <c r="C198" s="4" t="n">
         <v>55221</v>
       </c>
       <c r="D198" s="3"/>
@@ -7413,7 +7413,7 @@
       <c r="B199" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C199" s="5" t="n">
+      <c r="C199" s="4" t="n">
         <v>55426</v>
       </c>
       <c r="D199" s="3"/>
@@ -7445,7 +7445,7 @@
       <c r="B200" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="C200" s="5" t="n">
+      <c r="C200" s="4" t="n">
         <v>55428</v>
       </c>
       <c r="D200" s="3"/>
@@ -7477,7 +7477,7 @@
       <c r="B201" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C201" s="5" t="n">
+      <c r="C201" s="4" t="n">
         <v>55307</v>
       </c>
       <c r="D201" s="3"/>
@@ -7509,7 +7509,7 @@
       <c r="B202" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C202" s="5" t="n">
+      <c r="C202" s="4" t="n">
         <v>55012</v>
       </c>
       <c r="D202" s="3"/>
@@ -7541,7 +7541,7 @@
       <c r="B203" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C203" s="5" t="n">
+      <c r="C203" s="4" t="n">
         <v>55018</v>
       </c>
       <c r="D203" s="3"/>
@@ -7569,7 +7569,7 @@
     <row r="204" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="3"/>
       <c r="B204" s="3"/>
-      <c r="C204" s="5"/>
+      <c r="C204" s="4"/>
       <c r="D204" s="3"/>
       <c r="E204" s="3"/>
       <c r="F204" s="3"/>
@@ -7599,7 +7599,7 @@
       <c r="B205" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C205" s="5" t="n">
+      <c r="C205" s="4" t="n">
         <v>55018</v>
       </c>
       <c r="D205" s="3"/>
@@ -7631,7 +7631,7 @@
       <c r="B206" s="3" t="s">
         <v>227</v>
       </c>
-      <c r="C206" s="5" t="n">
+      <c r="C206" s="4" t="n">
         <v>55018</v>
       </c>
       <c r="D206" s="3"/>
@@ -7663,7 +7663,7 @@
       <c r="B207" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C207" s="5" t="n">
+      <c r="C207" s="4" t="n">
         <v>55018</v>
       </c>
       <c r="D207" s="3"/>
@@ -7695,7 +7695,7 @@
       <c r="B208" s="3" t="s">
         <v>233</v>
       </c>
-      <c r="C208" s="5" t="n">
+      <c r="C208" s="4" t="n">
         <v>55014</v>
       </c>
       <c r="D208" s="3"/>
@@ -7727,7 +7727,7 @@
       <c r="B209" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="C209" s="5" t="n">
+      <c r="C209" s="4" t="n">
         <v>55014</v>
       </c>
       <c r="D209" s="3"/>
@@ -7759,7 +7759,7 @@
       <c r="B210" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="C210" s="5" t="n">
+      <c r="C210" s="4" t="n">
         <v>55014</v>
       </c>
       <c r="D210" s="3"/>
@@ -7791,7 +7791,7 @@
       <c r="B211" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C211" s="5" t="n">
+      <c r="C211" s="4" t="n">
         <v>55014</v>
       </c>
       <c r="D211" s="3"/>
@@ -7823,7 +7823,7 @@
       <c r="B212" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C212" s="5" t="n">
+      <c r="C212" s="4" t="n">
         <v>55018</v>
       </c>
       <c r="D212" s="3"/>
@@ -7855,7 +7855,7 @@
       <c r="B213" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C213" s="5"/>
+      <c r="C213" s="4"/>
       <c r="D213" s="3"/>
       <c r="E213" s="3"/>
       <c r="F213" s="3"/>
@@ -7885,7 +7885,7 @@
       <c r="B214" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C214" s="5" t="n">
+      <c r="C214" s="4" t="n">
         <v>55020</v>
       </c>
       <c r="D214" s="3"/>
@@ -7917,7 +7917,7 @@
       <c r="B215" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="C215" s="5" t="n">
+      <c r="C215" s="4" t="n">
         <v>55020</v>
       </c>
       <c r="D215" s="3"/>
@@ -7949,7 +7949,7 @@
       <c r="B216" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C216" s="5" t="n">
+      <c r="C216" s="4" t="n">
         <v>55020</v>
       </c>
       <c r="D216" s="3"/>
@@ -7981,7 +7981,7 @@
       <c r="B217" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C217" s="5" t="n">
+      <c r="C217" s="4" t="n">
         <v>55101</v>
       </c>
       <c r="D217" s="3"/>
@@ -8013,7 +8013,7 @@
       <c r="B218" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C218" s="5" t="n">
+      <c r="C218" s="4" t="n">
         <v>55202</v>
       </c>
       <c r="D218" s="3"/>
@@ -8045,7 +8045,7 @@
       <c r="B219" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C219" s="5" t="n">
+      <c r="C219" s="4" t="n">
         <v>55208</v>
       </c>
       <c r="D219" s="3"/>
@@ -8077,7 +8077,7 @@
       <c r="B220" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C220" s="5" t="n">
+      <c r="C220" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D220" s="3"/>
@@ -8109,7 +8109,7 @@
       <c r="B221" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C221" s="5" t="n">
+      <c r="C221" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D221" s="3"/>
@@ -8141,7 +8141,7 @@
       <c r="B222" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C222" s="5" t="n">
+      <c r="C222" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D222" s="3"/>
@@ -8173,7 +8173,7 @@
       <c r="B223" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C223" s="5" t="n">
+      <c r="C223" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D223" s="3"/>
@@ -8205,7 +8205,7 @@
       <c r="B224" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C224" s="5" t="n">
+      <c r="C224" s="4" t="n">
         <v>55210</v>
       </c>
       <c r="D224" s="3"/>
@@ -8237,7 +8237,7 @@
       <c r="B225" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C225" s="5" t="n">
+      <c r="C225" s="4" t="n">
         <v>55216</v>
       </c>
       <c r="D225" s="3"/>
@@ -8269,7 +8269,7 @@
       <c r="B226" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C226" s="5" t="n">
+      <c r="C226" s="4" t="n">
         <v>55216</v>
       </c>
       <c r="D226" s="3"/>
@@ -8301,7 +8301,7 @@
       <c r="B227" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C227" s="5" t="n">
+      <c r="C227" s="4" t="n">
         <v>55218</v>
       </c>
       <c r="D227" s="3"/>
@@ -8333,7 +8333,7 @@
       <c r="B228" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C228" s="5" t="n">
+      <c r="C228" s="4" t="n">
         <v>55228</v>
       </c>
       <c r="D228" s="3"/>
@@ -8365,7 +8365,7 @@
       <c r="B229" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C229" s="5" t="n">
+      <c r="C229" s="4" t="n">
         <v>55228</v>
       </c>
       <c r="D229" s="3"/>
@@ -8397,7 +8397,7 @@
       <c r="B230" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C230" s="5" t="n">
+      <c r="C230" s="4" t="n">
         <v>55228</v>
       </c>
       <c r="D230" s="3"/>
@@ -8429,7 +8429,7 @@
       <c r="B231" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C231" s="5" t="n">
+      <c r="C231" s="4" t="n">
         <v>55107</v>
       </c>
       <c r="D231" s="3"/>
@@ -8461,7 +8461,7 @@
       <c r="B232" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C232" s="5" t="n">
+      <c r="C232" s="4" t="n">
         <v>55201</v>
       </c>
       <c r="D232" s="3"/>
@@ -8493,7 +8493,7 @@
       <c r="B233" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C233" s="5" t="n">
+      <c r="C233" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D233" s="3"/>
@@ -8525,7 +8525,7 @@
       <c r="B234" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C234" s="5" t="n">
+      <c r="C234" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D234" s="3"/>
@@ -8557,7 +8557,7 @@
       <c r="B235" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C235" s="5" t="n">
+      <c r="C235" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D235" s="3"/>
@@ -8589,7 +8589,7 @@
       <c r="B236" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C236" s="5" t="n">
+      <c r="C236" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D236" s="3"/>
@@ -8621,7 +8621,7 @@
       <c r="B237" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C237" s="5" t="n">
+      <c r="C237" s="4" t="n">
         <v>55215</v>
       </c>
       <c r="D237" s="3"/>
@@ -8653,7 +8653,7 @@
       <c r="B238" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="C238" s="5" t="n">
+      <c r="C238" s="4" t="n">
         <v>55228</v>
       </c>
       <c r="D238" s="3"/>

</xml_diff>